<commit_message>
[DOC] update release notes and readme for rc tag (#202)
* update release notes and readme for rc tag

* Add files via upload

* Manually stamping after test plan file update

* Manually stamping after test plan file update
</commit_message>
<xml_diff>
--- a/docs/AdamsBridge_TestPlan.xlsx
+++ b/docs/AdamsBridge_TestPlan.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/mojtabab_microsoft_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michnorris\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{C84845F9-CD33-4E93-858C-BC98E6A37371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D1F525D-0313-497D-9F90-6764D7BECA82}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8EE2E3-1E49-4B69-831A-84C9CFEA6265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2058A31A-58CD-4C0E-B892-9560631454C3}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2058A31A-58CD-4C0E-B892-9560631454C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Adams Bridge" sheetId="1" r:id="rId1"/>
+    <sheet name="ML-KEM" sheetId="2" r:id="rId1"/>
+    <sheet name="ML-DSA" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="118">
   <si>
     <t>Test Category</t>
   </si>
@@ -330,13 +331,112 @@
   </si>
   <si>
     <t xml:space="preserve">Checking the lint </t>
+  </si>
+  <si>
+    <t>Directed Encaps KATs (tb)</t>
+  </si>
+  <si>
+    <t>Directed Keygen+Decaps KATs (tb)</t>
+  </si>
+  <si>
+    <t>Directed Decaps KATs (tb)</t>
+  </si>
+  <si>
+    <t>Directed Keygen+Decaps KATs (smoke tests)</t>
+  </si>
+  <si>
+    <t>Directed Encaps KATs (smoke tests)</t>
+  </si>
+  <si>
+    <t>Directed Decaps KATs (smoke tests)</t>
+  </si>
+  <si>
+    <t>selected operation</t>
+  </si>
+  <si>
+    <t>order of operation</t>
+  </si>
+  <si>
+    <t>input data</t>
+  </si>
+  <si>
+    <t>Randomly select keygen/encap/decap and verify using reference model</t>
+  </si>
+  <si>
+    <t>Zero-seed KAT</t>
+  </si>
+  <si>
+    <t>seed = 0</t>
+  </si>
+  <si>
+    <t>Run keygen with all-zero seed and validate against known behavior</t>
+  </si>
+  <si>
+    <t>Assert zeroize simultaneously with keygen, encaps, or decap</t>
+  </si>
+  <si>
+    <t>kv interaction</t>
+  </si>
+  <si>
+    <t>Perform key generation, Encaps or Decaps with the seed sourced from KV, ensuring the secret asset remains hidden from firmware.</t>
+  </si>
+  <si>
+    <t>encapsulation with invalid ek</t>
+  </si>
+  <si>
+    <t>Set a 12b coefficient value in the EK to &gt;= MLKEM Q</t>
+  </si>
+  <si>
+    <t>decapsulation with invalid dk</t>
+  </si>
+  <si>
+    <t>Bit flip on EK/hash portion of DK</t>
+  </si>
+  <si>
+    <t>Decaps rejection</t>
+  </si>
+  <si>
+    <t>valid ct from a different EK</t>
+  </si>
+  <si>
+    <t>Use a ciphertext from a different EK and ensure decapsulation fails (comparing with expected shared key)</t>
+  </si>
+  <si>
+    <t>Prevent partial key recovery</t>
+  </si>
+  <si>
+    <t>zeroize during kv access</t>
+  </si>
+  <si>
+    <t>fw read during kv access</t>
+  </si>
+  <si>
+    <t>Restrict fw access while kv assets exist</t>
+  </si>
+  <si>
+    <t>reading the API during the process</t>
+  </si>
+  <si>
+    <t>any unlock(excluding the regular valid output) clears the API content</t>
+  </si>
+  <si>
+    <t>only valid signature unlocks the API and releases the content</t>
+  </si>
+  <si>
+    <t>scan_mode/debug</t>
+  </si>
+  <si>
+    <t>Unit Level TB</t>
+  </si>
+  <si>
+    <t>barrett reduction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -819,14 +919,459 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C500B135-D206-40C8-AD66-190B8CAE2D72}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="128" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="C20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2358D7B-DEAE-4F02-ABA1-0E276E6F0B9A}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
@@ -835,7 +1380,7 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -861,7 +1406,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -875,7 +1420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>10</v>
@@ -890,7 +1435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -904,7 +1449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>14</v>
@@ -919,7 +1464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>16</v>
       </c>
@@ -933,7 +1478,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>18</v>
@@ -948,7 +1493,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>20</v>
@@ -963,7 +1508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>22</v>
       </c>
@@ -977,7 +1522,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45">
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="7" t="s">
         <v>24</v>
@@ -992,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -1006,7 +1551,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>31</v>
@@ -1019,7 +1564,7 @@
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +1575,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>36</v>
@@ -1043,7 +1588,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -1054,7 +1599,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4" t="s">
         <v>40</v>
@@ -1067,7 +1612,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="30">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>42</v>
       </c>
@@ -1078,20 +1623,20 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>46</v>
@@ -1106,7 +1651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -1120,19 +1665,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4" t="s">
         <v>52</v>
@@ -1145,7 +1690,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>54</v>
       </c>
@@ -1156,7 +1701,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="45">
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="7" t="s">
         <v>56</v>
@@ -1167,7 +1712,7 @@
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>58</v>
       </c>
@@ -1175,7 +1720,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
         <v>60</v>
@@ -1186,12 +1731,12 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="60">
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="7" t="s">
         <v>63</v>
@@ -1202,7 +1747,7 @@
       </c>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>65</v>
       </c>
@@ -1210,7 +1755,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
         <v>67</v>
@@ -1221,7 +1766,7 @@
       </c>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>69</v>
       </c>
@@ -1229,7 +1774,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
         <v>71</v>
@@ -1240,7 +1785,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>73</v>
       </c>
@@ -1248,7 +1793,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>75</v>
@@ -1259,7 +1804,7 @@
       </c>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>77</v>
       </c>
@@ -1267,7 +1812,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>79</v>
@@ -1278,7 +1823,7 @@
       </c>
       <c r="E39" s="4"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>81</v>
       </c>
@@ -1286,7 +1831,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
         <v>83</v>

</xml_diff>